<commit_message>
Add ons in list
</commit_message>
<xml_diff>
--- a/Fruit Name.xlsx
+++ b/Fruit Name.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Facilities Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\Documents\GitHub\TestGithub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Color</t>
   </si>
@@ -52,6 +52,33 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Dark Green</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Bottle Green</t>
+  </si>
+  <si>
+    <t>Kiwi</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Black Currant</t>
   </si>
 </sst>
 </file>
@@ -367,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,6 +462,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>